<commit_message>
Segundo happy test validado
</commit_message>
<xml_diff>
--- a/Modelo Test Cases.xlsx
+++ b/Modelo Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Ch2_Etp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AF0384-862D-45C1-9FBA-BD0F89624882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52CF934-5300-4ACD-8A33-70FBE74F3C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Happy Path" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -130,6 +130,19 @@
   </si>
   <si>
     <t>PASÓ</t>
+  </si>
+  <si>
+    <t>Agregar un item a el carrito</t>
+  </si>
+  <si>
+    <t>Ir a la página del sitio</t>
+  </si>
+  <si>
+    <t>1. Hacer hover en la tarjeta de algún item
+2. Hacer click en "Add to cart"</t>
+  </si>
+  <si>
+    <t>Aparece un modal con la notificación de que el item fue agregado al carrito.</t>
   </si>
 </sst>
 </file>
@@ -266,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -311,6 +324,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -598,16 +623,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="17" customWidth="1"/>
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
@@ -678,23 +703,35 @@
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="B3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -704,14 +741,27 @@
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>